<commit_message>
inicio de sesion en portal claro
</commit_message>
<xml_diff>
--- a/src/routes/tuya/Formato de Campos Nuevo Colaborador.xlsx
+++ b/src/routes/tuya/Formato de Campos Nuevo Colaborador.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eapla\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A147FEC-42CE-4CCC-95F5-0DEF9712A060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44908CD2-3710-422F-9128-861D1AC8552C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
   <si>
     <t>Empresa</t>
   </si>
@@ -528,7 +529,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -559,19 +560,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -852,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
-      <selection activeCell="BZ16" sqref="BZ16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -963,10 +958,10 @@
       <c r="O1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="13" t="s">
         <v>125</v>
       </c>
       <c r="R1" s="8" t="s">
@@ -1041,7 +1036,7 @@
       <c r="AO1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AP1" s="1" t="s">
         <v>126</v>
       </c>
       <c r="AQ1" s="1" t="s">
@@ -1202,10 +1197,10 @@
       <c r="L2" s="6">
         <v>123456789</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>119</v>
       </c>
       <c r="O2" s="6">
@@ -1214,10 +1209,10 @@
       <c r="P2" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="10" t="s">
         <v>120</v>
       </c>
       <c r="S2" t="s">
@@ -1414,12 +1409,252 @@
       </c>
     </row>
     <row r="3" spans="1:82">
-      <c r="A3" s="3"/>
-      <c r="S3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="AW3" s="6"/>
-      <c r="AX3" s="10"/>
-      <c r="CB3" s="5"/>
+      <c r="A3" s="3">
+        <v>44965</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="3">
+        <v>35960</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="6">
+        <v>123456789</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="O3" s="6">
+        <v>123456789</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="S3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" t="s">
+        <v>76</v>
+      </c>
+      <c r="U3" t="s">
+        <v>73</v>
+      </c>
+      <c r="V3" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD3">
+        <v>2</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF3">
+        <v>70008883</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>45141</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX3" s="3">
+        <v>45202</v>
+      </c>
+      <c r="AY3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>94</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>98</v>
+      </c>
+      <c r="BO3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>103</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB3" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>105</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="4" spans="1:82">
       <c r="A4" s="3"/>

</xml_diff>

<commit_message>
avance en pagina web
</commit_message>
<xml_diff>
--- a/src/routes/tuya/Formato de Campos Nuevo Colaborador.xlsx
+++ b/src/routes/tuya/Formato de Campos Nuevo Colaborador.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eapla\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44908CD2-3710-422F-9128-861D1AC8552C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F8514B-D2FF-4AC8-8F56-66050164799A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="360" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="165">
   <si>
     <t>Empresa</t>
   </si>
@@ -421,21 +420,140 @@
   </si>
   <si>
     <t>antioquita</t>
+  </si>
+  <si>
+    <t>Esteban</t>
+  </si>
+  <si>
+    <t>Ciudad de Expedición</t>
+  </si>
+  <si>
+    <t>madrid</t>
+  </si>
+  <si>
+    <t>fusagasugá</t>
+  </si>
+  <si>
+    <t>Tipo de correo</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>Tipo de teléfono</t>
+  </si>
+  <si>
+    <t>número de télefono</t>
+  </si>
+  <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>people@gmail.com</t>
+  </si>
+  <si>
+    <t>sí</t>
+  </si>
+  <si>
+    <t>Nombres del familiar</t>
+  </si>
+  <si>
+    <t>Apellidos del familiar</t>
+  </si>
+  <si>
+    <t>vive con usted</t>
+  </si>
+  <si>
+    <t>depende de usted</t>
+  </si>
+  <si>
+    <t>Estudia actualmente</t>
+  </si>
+  <si>
+    <t>Estado de discapacidad</t>
+  </si>
+  <si>
+    <t>Lugar de emisión</t>
+  </si>
+  <si>
+    <t>Autoridad emisora</t>
+  </si>
+  <si>
+    <t>Fecha de caducidad</t>
+  </si>
+  <si>
+    <t>Genero del familiar</t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento del familiar</t>
+  </si>
+  <si>
+    <t>Contacto de emergencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parentesco </t>
+  </si>
+  <si>
+    <t>Movil</t>
+  </si>
+  <si>
+    <t>sol</t>
+  </si>
+  <si>
+    <t>hermana</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
+    <t>plata</t>
+  </si>
+  <si>
+    <t>madre</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>Parentesco del familiar</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>esteban</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/mm/yy"/>
-  </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,6 +606,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -524,54 +650,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD4"/>
+  <dimension ref="A1:CY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -865,304 +1001,387 @@
     <col min="11" max="11" width="22.5703125" customWidth="1"/>
     <col min="12" max="12" width="19.85546875" customWidth="1"/>
     <col min="13" max="17" width="29.7109375" customWidth="1"/>
-    <col min="18" max="18" width="22.5703125" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" customWidth="1"/>
-    <col min="23" max="24" width="40.140625" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125"/>
-    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="46.85546875" customWidth="1"/>
-    <col min="36" max="36" width="41.28515625" customWidth="1"/>
-    <col min="37" max="37" width="21.28515625" customWidth="1"/>
-    <col min="38" max="38" width="23.28515625" customWidth="1"/>
-    <col min="39" max="40" width="47.28515625" customWidth="1"/>
-    <col min="41" max="42" width="71.28515625" customWidth="1"/>
-    <col min="43" max="43" width="14.7109375" customWidth="1"/>
-    <col min="44" max="44" width="20.140625" customWidth="1"/>
-    <col min="45" max="45" width="24.42578125" customWidth="1"/>
-    <col min="46" max="46" width="20.140625" customWidth="1"/>
-    <col min="47" max="47" width="21.7109375" customWidth="1"/>
-    <col min="48" max="48" width="18" customWidth="1"/>
-    <col min="49" max="49" width="38.85546875" customWidth="1"/>
-    <col min="50" max="50" width="29.42578125" customWidth="1"/>
-    <col min="51" max="52" width="19.42578125" customWidth="1"/>
-    <col min="53" max="54" width="11.28515625" customWidth="1"/>
-    <col min="55" max="55" width="11.7109375" customWidth="1"/>
-    <col min="56" max="56" width="25" customWidth="1"/>
-    <col min="57" max="57" width="15" customWidth="1"/>
-    <col min="58" max="58" width="12.5703125" customWidth="1"/>
-    <col min="59" max="59" width="19.140625" customWidth="1"/>
-    <col min="60" max="60" width="15.5703125" customWidth="1"/>
-    <col min="64" max="64" width="25.5703125" customWidth="1"/>
-    <col min="68" max="68" width="27.5703125" customWidth="1"/>
-    <col min="69" max="69" width="27" customWidth="1"/>
-    <col min="70" max="70" width="22.5703125" customWidth="1"/>
-    <col min="71" max="71" width="14.140625" customWidth="1"/>
-    <col min="72" max="72" width="15.42578125" customWidth="1"/>
-    <col min="73" max="73" width="25.5703125" customWidth="1"/>
-    <col min="74" max="74" width="17.7109375" customWidth="1"/>
-    <col min="75" max="75" width="20.5703125" customWidth="1"/>
-    <col min="76" max="76" width="18.85546875" customWidth="1"/>
-    <col min="77" max="77" width="12.140625" customWidth="1"/>
-    <col min="78" max="78" width="17.5703125" customWidth="1"/>
-    <col min="79" max="79" width="21.28515625" customWidth="1"/>
-    <col min="80" max="80" width="9.7109375"/>
-    <col min="82" max="82" width="13.42578125" customWidth="1"/>
+    <col min="18" max="19" width="22.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" customWidth="1"/>
+    <col min="24" max="25" width="40.140625" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" customWidth="1"/>
+    <col min="31" max="31" width="21.28515625" customWidth="1"/>
+    <col min="32" max="32" width="21.85546875" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" customWidth="1"/>
+    <col min="37" max="37" width="17.5703125" customWidth="1"/>
+    <col min="38" max="38" width="25.5703125" customWidth="1"/>
+    <col min="39" max="40" width="17.5703125" customWidth="1"/>
+    <col min="41" max="41" width="22.28515625" customWidth="1"/>
+    <col min="42" max="42" width="21.5703125" customWidth="1"/>
+    <col min="43" max="43" width="28" customWidth="1"/>
+    <col min="44" max="44" width="17.5703125" customWidth="1"/>
+    <col min="45" max="45" width="19.28515625" customWidth="1"/>
+    <col min="46" max="46" width="22.42578125" customWidth="1"/>
+    <col min="47" max="47" width="25.140625" customWidth="1"/>
+    <col min="48" max="48" width="18.28515625" customWidth="1"/>
+    <col min="49" max="49" width="19.85546875" customWidth="1"/>
+    <col min="50" max="51" width="24.140625" customWidth="1"/>
+    <col min="52" max="52" width="35.42578125" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125"/>
+    <col min="54" max="54" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="46.85546875" customWidth="1"/>
+    <col min="57" max="57" width="41.28515625" customWidth="1"/>
+    <col min="58" max="58" width="21.28515625" customWidth="1"/>
+    <col min="59" max="59" width="23.28515625" customWidth="1"/>
+    <col min="60" max="61" width="47.28515625" customWidth="1"/>
+    <col min="62" max="63" width="71.28515625" customWidth="1"/>
+    <col min="64" max="64" width="14.7109375" customWidth="1"/>
+    <col min="65" max="65" width="20.140625" customWidth="1"/>
+    <col min="66" max="66" width="24.42578125" customWidth="1"/>
+    <col min="67" max="67" width="20.140625" customWidth="1"/>
+    <col min="68" max="68" width="21.7109375" customWidth="1"/>
+    <col min="69" max="69" width="18" customWidth="1"/>
+    <col min="70" max="70" width="38.85546875" customWidth="1"/>
+    <col min="71" max="71" width="29.42578125" customWidth="1"/>
+    <col min="72" max="73" width="19.42578125" customWidth="1"/>
+    <col min="74" max="75" width="11.28515625" customWidth="1"/>
+    <col min="76" max="76" width="11.7109375" customWidth="1"/>
+    <col min="77" max="77" width="25" customWidth="1"/>
+    <col min="78" max="78" width="15" customWidth="1"/>
+    <col min="79" max="79" width="12.5703125" customWidth="1"/>
+    <col min="80" max="80" width="19.140625" customWidth="1"/>
+    <col min="81" max="81" width="15.5703125" customWidth="1"/>
+    <col min="85" max="85" width="25.5703125" customWidth="1"/>
+    <col min="89" max="89" width="27.5703125" customWidth="1"/>
+    <col min="90" max="90" width="27" customWidth="1"/>
+    <col min="91" max="91" width="22.5703125" customWidth="1"/>
+    <col min="92" max="92" width="14.140625" customWidth="1"/>
+    <col min="93" max="93" width="15.42578125" customWidth="1"/>
+    <col min="94" max="94" width="25.5703125" customWidth="1"/>
+    <col min="95" max="95" width="17.7109375" customWidth="1"/>
+    <col min="96" max="96" width="20.5703125" customWidth="1"/>
+    <col min="97" max="97" width="18.85546875" customWidth="1"/>
+    <col min="98" max="98" width="12.140625" customWidth="1"/>
+    <col min="99" max="99" width="17.5703125" customWidth="1"/>
+    <col min="100" max="100" width="21.28515625" customWidth="1"/>
+    <col min="101" max="101" width="9.7109375"/>
+    <col min="103" max="103" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="15.75">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:103" ht="15.75">
+      <c r="A1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AH1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AI1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AK1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AW1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="BG1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="BR1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="BS1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="BT1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="BU1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="BV1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BW1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BX1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BY1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="CA1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="CB1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="BH1" s="9" t="s">
+      <c r="CC1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="CD1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="CE1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="CF1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="CG1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="CH1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="CI1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="CJ1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BP1" s="8" t="s">
+      <c r="CK1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BR1" s="9" t="s">
+      <c r="CM1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="BS1" s="9" t="s">
+      <c r="CN1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="BT1" s="9" t="s">
+      <c r="CO1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="BU1" s="9" t="s">
+      <c r="CP1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="BV1" s="9" t="s">
+      <c r="CQ1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BW1" s="9" t="s">
+      <c r="CR1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="BX1" s="9" t="s">
+      <c r="CS1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BY1" s="9" t="s">
+      <c r="CT1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="CA1" s="8" t="s">
+      <c r="CV1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="CB1" s="8" t="s">
+      <c r="CW1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="CD1" s="8" t="s">
+      <c r="CY1" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:82">
+    <row r="2" spans="1:103">
       <c r="A2" s="3">
-        <v>44965</v>
+        <v>80223</v>
       </c>
       <c r="B2" t="s">
         <v>69</v>
@@ -1174,10 +1393,10 @@
         <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -1194,223 +1413,277 @@
       <c r="K2" t="s">
         <v>118</v>
       </c>
-      <c r="L2" s="6">
-        <v>123456789</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="6">
-        <v>123456789</v>
-      </c>
-      <c r="P2" s="6" t="s">
+      <c r="O2" s="5">
+        <v>123456</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" t="s">
         <v>75</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>76</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>73</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>77</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>78</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>79</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>73</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE2">
+        <v>3154789875</v>
+      </c>
+      <c r="AF2" t="s">
         <v>80</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AG2" t="s">
         <v>73</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AH2" t="s">
         <v>128</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AI2" t="s">
         <v>127</v>
       </c>
-      <c r="AD2">
+      <c r="AJ2">
         <v>2</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AK2" t="s">
         <v>80</v>
       </c>
-      <c r="AF2">
+      <c r="AL2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN2">
+        <v>3214569878</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AZ2" s="3">
+        <v>28858</v>
+      </c>
+      <c r="BA2">
         <v>70008883</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="BB2" s="3">
         <v>45141</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="BC2" t="s">
         <v>69</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="BD2" t="s">
         <v>81</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="BE2" t="s">
         <v>82</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="BF2" t="s">
         <v>83</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="BG2" t="s">
         <v>84</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="BH2" t="s">
         <v>85</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="BI2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="BJ2" t="s">
         <v>86</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="BK2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="BL2" t="s">
         <v>87</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="BM2" t="s">
         <v>88</v>
       </c>
-      <c r="AS2">
+      <c r="BN2">
         <v>1</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="BO2" t="s">
         <v>89</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BP2" t="s">
         <v>90</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BQ2" t="s">
         <v>91</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BR2" t="s">
         <v>99</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="BS2" s="3">
         <v>45202</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="BT2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BU2" t="s">
         <v>93</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BV2" t="s">
         <v>94</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BW2" t="s">
         <v>94</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BX2" t="s">
         <v>95</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BY2" t="s">
         <v>96</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BZ2" t="s">
         <v>74</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="CA2" t="s">
         <v>74</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="CB2" t="s">
         <v>96</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="CC2" t="s">
         <v>97</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="CD2" t="s">
         <v>96</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="CE2" t="s">
         <v>96</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="CF2" t="s">
         <v>96</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="CG2" t="s">
         <v>96</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="CH2" t="s">
         <v>96</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="CI2" t="s">
         <v>98</v>
       </c>
-      <c r="BO2" s="6" t="s">
+      <c r="CJ2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="CK2" t="s">
         <v>92</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="CL2" t="s">
         <v>89</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="CM2" t="s">
         <v>89</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="CN2" t="s">
         <v>100</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="CO2" t="s">
         <v>89</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="CP2" t="s">
         <v>89</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="CQ2" t="s">
         <v>89</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CR2" t="s">
         <v>101</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CS2" t="s">
         <v>89</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CT2" t="s">
         <v>102</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CU2" t="s">
         <v>103</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CV2" t="s">
         <v>104</v>
       </c>
-      <c r="CB2" s="5">
+      <c r="CW2" s="4">
         <v>1000000</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CX2" t="s">
         <v>105</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CY2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:82">
+    <row r="3" spans="1:103">
       <c r="A3" s="3">
-        <v>44965</v>
+        <v>80223</v>
       </c>
       <c r="B3" t="s">
         <v>69</v>
@@ -1442,227 +1715,288 @@
       <c r="K3" t="s">
         <v>118</v>
       </c>
-      <c r="L3" s="6">
-        <v>123456789</v>
-      </c>
-      <c r="M3" s="10" t="s">
+      <c r="L3" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="O3" s="6">
-        <v>123456789</v>
-      </c>
-      <c r="P3" s="6" t="s">
+      <c r="O3" s="5">
+        <v>123454545</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3" t="s">
         <v>75</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>76</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>73</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>77</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>78</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>79</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>73</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB3" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE3">
+        <v>3154789875</v>
+      </c>
+      <c r="AF3" t="s">
         <v>80</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AG3" t="s">
         <v>73</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AH3" t="s">
         <v>128</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AI3" t="s">
         <v>127</v>
       </c>
-      <c r="AD3">
+      <c r="AJ3">
         <v>2</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AK3" t="s">
         <v>80</v>
       </c>
-      <c r="AF3">
+      <c r="AL3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN3">
+        <v>3214569878</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>157</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AX3" s="3">
+        <v>45993</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AZ3" s="3">
+        <v>28858</v>
+      </c>
+      <c r="BA3">
         <v>70008883</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="BB3" s="3">
         <v>45141</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="BC3" t="s">
         <v>69</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="BD3" t="s">
         <v>81</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="BE3" t="s">
         <v>82</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="BF3" t="s">
         <v>83</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="BG3" t="s">
         <v>84</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="BH3" t="s">
         <v>85</v>
       </c>
-      <c r="AN3" s="6" t="s">
+      <c r="BI3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="BJ3" t="s">
         <v>86</v>
       </c>
-      <c r="AP3" s="6" t="s">
+      <c r="BK3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="BL3" t="s">
         <v>87</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="BM3" t="s">
         <v>88</v>
       </c>
-      <c r="AS3">
+      <c r="BN3">
         <v>1</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="BO3" t="s">
         <v>89</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="BP3" t="s">
         <v>90</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="BQ3" t="s">
         <v>91</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="BR3" t="s">
         <v>99</v>
       </c>
-      <c r="AX3" s="3">
+      <c r="BS3" s="3">
         <v>45202</v>
       </c>
-      <c r="AY3" s="6" t="s">
+      <c r="BT3" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BU3" t="s">
         <v>93</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BV3" t="s">
         <v>94</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BW3" t="s">
         <v>94</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BX3" t="s">
         <v>95</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BY3" t="s">
         <v>96</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BZ3" t="s">
         <v>74</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="CA3" t="s">
         <v>74</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="CB3" t="s">
         <v>96</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="CC3" t="s">
         <v>97</v>
       </c>
-      <c r="BI3" t="s">
+      <c r="CD3" t="s">
         <v>96</v>
       </c>
-      <c r="BJ3" t="s">
+      <c r="CE3" t="s">
         <v>96</v>
       </c>
-      <c r="BK3" t="s">
+      <c r="CF3" t="s">
         <v>96</v>
       </c>
-      <c r="BL3" t="s">
+      <c r="CG3" t="s">
         <v>96</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="CH3" t="s">
         <v>96</v>
       </c>
-      <c r="BN3" t="s">
+      <c r="CI3" t="s">
         <v>98</v>
       </c>
-      <c r="BO3" s="6" t="s">
+      <c r="CJ3" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="BP3" t="s">
+      <c r="CK3" t="s">
         <v>92</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="CL3" t="s">
         <v>89</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="CM3" t="s">
         <v>89</v>
       </c>
-      <c r="BS3" t="s">
+      <c r="CN3" t="s">
         <v>100</v>
       </c>
-      <c r="BT3" t="s">
+      <c r="CO3" t="s">
         <v>89</v>
       </c>
-      <c r="BU3" t="s">
+      <c r="CP3" t="s">
         <v>89</v>
       </c>
-      <c r="BV3" t="s">
+      <c r="CQ3" t="s">
         <v>89</v>
       </c>
-      <c r="BW3" t="s">
+      <c r="CR3" t="s">
         <v>101</v>
       </c>
-      <c r="BX3" t="s">
+      <c r="CS3" t="s">
         <v>89</v>
       </c>
-      <c r="BY3" t="s">
+      <c r="CT3" t="s">
         <v>102</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="CU3" t="s">
         <v>103</v>
       </c>
-      <c r="CA3" t="s">
+      <c r="CV3" t="s">
         <v>104</v>
       </c>
-      <c r="CB3" s="5">
+      <c r="CW3" s="4">
         <v>1000000</v>
       </c>
-      <c r="CC3" t="s">
+      <c r="CX3" t="s">
         <v>105</v>
       </c>
-      <c r="CD3" t="s">
+      <c r="CY3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:82">
-      <c r="A4" s="3"/>
-      <c r="G4" s="6"/>
-      <c r="AX4" s="4"/>
-      <c r="CB4" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AB2" r:id="rId1" xr:uid="{B685FF90-B14C-4810-AC81-CF740EDCE3BB}"/>
+    <hyperlink ref="AB3" r:id="rId2" xr:uid="{246D9536-5B09-4B48-BA37-B1C6FFD6402F}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrego acondicionamiento de las fechas
</commit_message>
<xml_diff>
--- a/src/routes/tuya/Formato de Campos Nuevo Colaborador.xlsx
+++ b/src/routes/tuya/Formato de Campos Nuevo Colaborador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eapla\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F14D3-348E-4FA0-97EE-CA9119FE505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC0B3A6-3B61-45A4-8A37-4887A9866C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1590" windowWidth="18330" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26775" yWindow="5490" windowWidth="18330" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="172">
   <si>
     <t>Empresa</t>
   </si>
@@ -371,12 +371,6 @@
     <t>Nivel_18_SBF (4000018)</t>
   </si>
   <si>
-    <t>leandro</t>
-  </si>
-  <si>
-    <t>garcia</t>
-  </si>
-  <si>
     <t>colombia</t>
   </si>
   <si>
@@ -398,9 +392,6 @@
     <t>Número de Documento</t>
   </si>
   <si>
-    <t>hols</t>
-  </si>
-  <si>
     <t>Fecha de Expedición</t>
   </si>
   <si>
@@ -542,35 +533,34 @@
     <t>miguel</t>
   </si>
   <si>
-    <t>stiven</t>
-  </si>
-  <si>
-    <t>lomas ageas</t>
-  </si>
-  <si>
-    <t>sergi</t>
-  </si>
-  <si>
-    <t>laguna</t>
+    <t>ANTONIA</t>
+  </si>
+  <si>
+    <t>GOMEZ</t>
+  </si>
+  <si>
+    <t>ALEJANDRO</t>
+  </si>
+  <si>
+    <t>MALDONADO</t>
+  </si>
+  <si>
+    <t>CR7</t>
+  </si>
+  <si>
+    <t>SIUUUUUU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -699,18 +689,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -719,35 +709,32 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1038,7 +1025,7 @@
   <dimension ref="A1:DC4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1125,7 +1112,7 @@
   <sheetData>
     <row r="1" spans="1:107" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1161,25 +1148,25 @@
         <v>10</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>107</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="Q1" s="12" t="s">
-        <v>122</v>
+      <c r="Q1" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>12</v>
@@ -1203,19 +1190,19 @@
         <v>18</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AF1" s="7" t="s">
         <v>19</v>
@@ -1236,49 +1223,49 @@
         <v>23</v>
       </c>
       <c r="AL1" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AM1" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AN1" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AO1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AT1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="AQ1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AU1" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AV1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="AT1" s="7" t="s">
+      <c r="AW1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AU1" s="7" t="s">
+      <c r="AX1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AV1" s="7" t="s">
+      <c r="AY1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AW1" s="7" t="s">
+      <c r="AZ1" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="AX1" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="AY1" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="AZ1" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="BA1" s="7" t="s">
         <v>24</v>
@@ -1311,7 +1298,7 @@
         <v>30</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>31</v>
@@ -1368,7 +1355,7 @@
         <v>46</v>
       </c>
       <c r="CD1" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="CE1" s="7" t="s">
         <v>47</v>
@@ -1389,7 +1376,7 @@
         <v>52</v>
       </c>
       <c r="CK1" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="CL1" s="7" t="s">
         <v>54</v>
@@ -1437,10 +1424,10 @@
         <v>67</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="DB1" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="DC1" s="7" t="s">
         <v>68</v>
@@ -1460,49 +1447,49 @@
         <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
       </c>
       <c r="H2" s="3">
-        <v>35960</v>
+        <v>35230</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
-      </c>
-      <c r="L2" s="13">
-        <v>1000000016</v>
+        <v>154</v>
+      </c>
+      <c r="L2" s="12">
+        <v>2000001100</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="O2" s="13">
-        <v>1000000016</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>121</v>
+        <v>112</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="12">
+        <v>2000001100</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>42169</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="T2" t="s">
         <v>75</v>
@@ -1526,16 +1513,16 @@
         <v>73</v>
       </c>
       <c r="AA2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="AC2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AD2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AE2">
         <v>3154789875</v>
@@ -1547,10 +1534,10 @@
         <v>73</v>
       </c>
       <c r="AH2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AI2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AJ2">
         <v>2</v>
@@ -1559,37 +1546,37 @@
         <v>80</v>
       </c>
       <c r="AL2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AM2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AN2">
         <v>3214569878</v>
       </c>
       <c r="AO2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS2" t="s">
         <v>149</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AT2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY2" t="s">
         <v>150</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>153</v>
       </c>
       <c r="AZ2" s="3">
         <v>28858</v>
@@ -1598,7 +1585,7 @@
         <v>70008883</v>
       </c>
       <c r="BB2" s="3">
-        <v>45141</v>
+        <v>45202</v>
       </c>
       <c r="BC2" t="s">
         <v>69</v>
@@ -1649,7 +1636,7 @@
         <v>99</v>
       </c>
       <c r="BS2" s="3">
-        <v>45202</v>
+        <v>45263</v>
       </c>
       <c r="BT2" s="5" t="s">
         <v>89</v>
@@ -1682,7 +1669,7 @@
         <v>97</v>
       </c>
       <c r="CD2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="CE2" t="s">
         <v>96</v>
@@ -1705,8 +1692,8 @@
       <c r="CK2" t="s">
         <v>100</v>
       </c>
-      <c r="CL2" s="18" t="s">
-        <v>155</v>
+      <c r="CL2" s="17" t="s">
+        <v>152</v>
       </c>
       <c r="CM2" t="s">
         <v>92</v>
@@ -1751,10 +1738,10 @@
         <v>105</v>
       </c>
       <c r="DA2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="DB2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DC2" t="s">
         <v>106</v>
@@ -1774,49 +1761,49 @@
         <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="G3" t="s">
         <v>72</v>
       </c>
       <c r="H3" s="3">
-        <v>35960</v>
+        <v>35230</v>
       </c>
       <c r="I3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" t="s">
         <v>114</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" s="12">
+        <v>2000000101</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" s="12">
+        <v>2000000101</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>42169</v>
+      </c>
+      <c r="R3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="13">
-        <v>1000000015</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="O3" s="13">
-        <v>1000000015</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>126</v>
+      <c r="S3" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="T3" t="s">
         <v>75</v>
@@ -1840,16 +1827,16 @@
         <v>73</v>
       </c>
       <c r="AA3" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB3" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="AC3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AD3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AE3">
         <v>3154789875</v>
@@ -1861,10 +1848,10 @@
         <v>73</v>
       </c>
       <c r="AH3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AI3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AJ3">
         <v>2</v>
@@ -1873,38 +1860,38 @@
         <v>80</v>
       </c>
       <c r="AL3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AM3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AN3">
         <v>3214569878</v>
       </c>
       <c r="AO3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS3" t="s">
         <v>149</v>
       </c>
-      <c r="AP3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>152</v>
-      </c>
       <c r="AT3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AU3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AX3" s="3"/>
       <c r="AY3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AZ3" s="3">
         <v>28858</v>
@@ -1913,7 +1900,7 @@
         <v>70008883</v>
       </c>
       <c r="BB3" s="3">
-        <v>45141</v>
+        <v>45202</v>
       </c>
       <c r="BC3" t="s">
         <v>69</v>
@@ -1964,7 +1951,7 @@
         <v>99</v>
       </c>
       <c r="BS3" s="3">
-        <v>45202</v>
+        <v>45263</v>
       </c>
       <c r="BT3" s="5" t="s">
         <v>89</v>
@@ -1997,7 +1984,7 @@
         <v>97</v>
       </c>
       <c r="CD3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="CE3" t="s">
         <v>96</v>
@@ -2020,8 +2007,8 @@
       <c r="CK3" t="s">
         <v>100</v>
       </c>
-      <c r="CL3" s="18" t="s">
-        <v>155</v>
+      <c r="CL3" s="17" t="s">
+        <v>152</v>
       </c>
       <c r="CM3" t="s">
         <v>92</v>
@@ -2066,10 +2053,10 @@
         <v>105</v>
       </c>
       <c r="DA3" t="s">
+        <v>162</v>
+      </c>
+      <c r="DB3" t="s">
         <v>165</v>
-      </c>
-      <c r="DB3" t="s">
-        <v>168</v>
       </c>
       <c r="DC3" t="s">
         <v>106</v>
@@ -2089,49 +2076,49 @@
         <v>71</v>
       </c>
       <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" t="s">
         <v>171</v>
-      </c>
-      <c r="F4" t="s">
-        <v>172</v>
       </c>
       <c r="G4" t="s">
         <v>72</v>
       </c>
       <c r="H4" s="3">
-        <v>35960</v>
+        <v>35230</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K4" t="s">
-        <v>157</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1000000025</v>
+        <v>154</v>
+      </c>
+      <c r="L4" s="12">
+        <v>2000000102</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="O4" s="13">
-        <v>1000000025</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>121</v>
+        <v>112</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="O4" s="12">
+        <v>2000000102</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>42169</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="S4" s="14" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="T4" t="s">
         <v>75</v>
@@ -2155,16 +2142,16 @@
         <v>73</v>
       </c>
       <c r="AA4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB4" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
+      </c>
+      <c r="AB4" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="AC4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AD4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AE4">
         <v>3154789875</v>
@@ -2176,10 +2163,10 @@
         <v>73</v>
       </c>
       <c r="AH4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AI4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AJ4">
         <v>2</v>
@@ -2188,37 +2175,37 @@
         <v>80</v>
       </c>
       <c r="AL4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AM4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AN4">
         <v>3214569878</v>
       </c>
       <c r="AO4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS4" t="s">
         <v>149</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AT4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY4" t="s">
         <v>150</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>153</v>
       </c>
       <c r="AZ4" s="3">
         <v>28858</v>
@@ -2227,7 +2214,7 @@
         <v>70008883</v>
       </c>
       <c r="BB4" s="3">
-        <v>45141</v>
+        <v>45202</v>
       </c>
       <c r="BC4" t="s">
         <v>69</v>
@@ -2278,7 +2265,7 @@
         <v>99</v>
       </c>
       <c r="BS4" s="3">
-        <v>45202</v>
+        <v>45263</v>
       </c>
       <c r="BT4" s="5" t="s">
         <v>89</v>
@@ -2311,7 +2298,7 @@
         <v>97</v>
       </c>
       <c r="CD4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="CE4" t="s">
         <v>96</v>
@@ -2334,8 +2321,8 @@
       <c r="CK4" t="s">
         <v>100</v>
       </c>
-      <c r="CL4" s="18" t="s">
-        <v>155</v>
+      <c r="CL4" s="17" t="s">
+        <v>152</v>
       </c>
       <c r="CM4" t="s">
         <v>92</v>
@@ -2380,10 +2367,10 @@
         <v>105</v>
       </c>
       <c r="DA4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="DB4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="DC4" t="s">
         <v>106</v>

</xml_diff>